<commit_message>
Communication skills section added
Communication skills section added
</commit_message>
<xml_diff>
--- a/DS.xlsx
+++ b/DS.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.haleshappa\Desktop\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6B467C-236A-49F9-9A9B-9E51ADD4E448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B61EFE6-FD89-4071-A350-19C9C42124BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DS" sheetId="1" r:id="rId1"/>
+    <sheet name="Communication" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DS!$A$1:$D$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>https://new.express.adobe.com/id/urn:aaid:sc:AP:3e9a1cdf-d245-4bbd-8473-a13a22547c4d?category=search&amp;learn=creative-exercises</t>
   </si>
@@ -182,12 +183,6 @@
     <t xml:space="preserve">After 500 rejections, 23-year-old lands OpenAI WFH job, earns Rs 20 lakh monthly - India Today </t>
   </si>
   <si>
-    <t xml:space="preserve">PowerBI - today I created this. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=sIYKNMbb2v8 </t>
-  </si>
-  <si>
     <t>How to print Name, Mobile Number, Email id and Address in Python using "User input function"</t>
   </si>
   <si>
@@ -227,12 +222,134 @@
 https://www.linkedin.com/feed/update/urn:li:activity:7283665505956093952/?updateEntityUrn=urn%3Ali%3Afs_updateV2%3A%28urn%3Ali%3Aactivity%3A7283665505956093952%2CFEED_DETAIL%2CEMPTY%2CDEFAULT%2Cfalse%29&amp;originTrackingId=CAIY6TIwRCqtU%2F0Uj1ZgCw%3D%3D 
 https://www.linkedin.com/in/laxmi-rani-bodana-882436256/ </t>
   </si>
+  <si>
+    <t>https://www.youtube.com/@campusx-official</t>
+  </si>
+  <si>
+    <t>AI cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZftI2fEz0Fw&amp;list=PLKnIA16_Rmvbr7zKYQuBfsVkjoLcJgxHH</t>
+  </si>
+  <si>
+    <t>ML - Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=u1RKh1kQqaE&amp;list=PLKnIA16_Rmvb1RYR-iTA_hzckhdONtSW4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kq9Vmg5d7Sk&amp;list=PLKnIA16_RmvbR85fgbfVRKOiMokUKVupy</t>
+  </si>
+  <si>
+    <t>Pandas</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CpPLLp3snK4&amp;list=PLKnIA16_Rmvb-ToL3RQ_bwxG4_ND-0-DT</t>
+  </si>
+  <si>
+    <t>Numpy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qKvgh-1XIpE&amp;list=PLKnIA16_RmvZGK-NF2YovesQ96HfUrKEw</t>
+  </si>
+  <si>
+    <t>How To Learn Python For Data Science In 14 Days | Complete Roadmap With Learning Resources</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sIYKNMbb2v8</t>
+  </si>
+  <si>
+    <t>PowerBI</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Types of Communication
+Verbal Communication – Spoken words and language.
+Non-verbal Communication – Body language, gestures, facial expressions.
+Written Communication – Emails, texts, reports, and other written formats.</t>
+  </si>
+  <si>
+    <t>😠 Aggressive Behavior
+Aggression is described as a planned act of anger, often manifesting in the following ways:
+Classic Behaviors of Aggressive People:
+Blaming others
+Intimidating body language
+Demanding actions
+Raised voice
+Harsh personal language
+Verbal blowouts</t>
+  </si>
+  <si>
+    <t>🗣️ Communication Styles
+1. Assertive Communication
+Described with the prompts: how, when, where — suggesting that assertiveness involves thoughtful timing, context, and delivery.
+Associated with community and positive behavior, such as conducting a survey or offering a surprise.
+2.Submissive/Passive Communication
+     Characterized by being a polite or nice older person, implying deference and avoidance of conflict.
+3.Passive-Aggressive Communication
+     Combines elements of both passive and assertive styles, often indirect and contradictory.
+4.Target Audience or Persona
+The phrase “The Person to use is an Older-People-People” suggests that these communication styles may be observed or practiced by older individuals, or that the context involves engaging with older adults.</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>Day2</t>
+  </si>
+  <si>
+    <t>Day 4</t>
+  </si>
+  <si>
+    <t>👂 4 Levels of Listening
+Hear – Basic auditory perception.
+Seeing – Observing non-verbal cues.
+Feeling – Empathizing with the speaker.
+Thinking – Processing and reflecting on the message.
+🧍 Passive Communication
+Described as a style where individuals:
+Are unaware of their own thoughts and feelings.
+Tend to prioritize others' needs over their own.
+Classic Behaviors of Passive People:
+Do not express themselves openly.
+Stew on things (internalize emotions).
+Withdraw or go remote, possibly with unclear or indirect targeting (noted as “L-Targeting”).</t>
+  </si>
+  <si>
+    <t>🧍 WIISFM Behaviors
+These behaviors reflect a passive communication style, often summarized by the acronym WIISFM:
+Soft voice
+Overly agreeable, without asserting a personal point of view
+Avoidance
+Withdrawn body language
+Seeming unsure
+Beating around the bush
+Appearing helpless or hopeless
+⚠️ Negative Attitudes
+These are internal states that often accompany passive behavior:
+Lack of self-confidence and low self-esteem
+Lack of self-respect
+Self put-downs
+Negative thoughts and feelings about oneself
+Feelings of inferiority toward others
+Preference for others to control situations
+Guilt towards others
+Feeling deactivated (emotionally or socially disengaged)</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,8 +381,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFA60000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +400,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC189F7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,6 +454,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -360,7 +496,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -424,13 +560,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -472,14 +608,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4936534</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>46560</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>130380</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -502,7 +638,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3611880" y="8161020"/>
+          <a:off x="3611880" y="11765280"/>
           <a:ext cx="4867954" cy="6020640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -516,13 +652,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -586,13 +722,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>88095</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>5486400</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>1088893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -892,9 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -904,21 +1042,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -931,269 +1069,385 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>61</v>
+        <v>69</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>58</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="25" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="36" spans="1:2" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>58</v>
+      <c r="B38" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D31" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D37" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{212DBCA1-AF2C-43B2-9A85-0C433F902C1E}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{0631045F-4915-4FF9-B22B-80AE3126D5B0}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{A4676929-B8C3-4901-8FF5-0BDC3175050E}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{7B7FBE21-B5F8-4EE9-AE85-B2DAD57BCD63}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.linkedin.com/in/laxmi-rani-bodana-882436256/ " xr:uid="{C1C86E05-B6ED-4FCB-960C-C888FC35B72A}"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://github.com/patan-abubakar8" xr:uid="{3B8B51B6-AE2F-4A55-99FC-37BEC1D0E397}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{B2197619-6013-44FB-8DB8-8A25DDCA479F}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{702632EC-18ED-471F-8542-ECF8E4573F41}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{B169D8E7-AB76-4F00-BAB8-075FEA5BAA4D}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{15CD9701-331C-4586-B09C-B1A64C71A263}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{B168966D-89E8-4E55-904C-419DDFFE368D}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{9CB6C6C7-3513-4B06-A3B2-8F63805A5AD0}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{D20CA113-FD85-4E12-AF69-2E6C5FD5E0C5}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{D306E866-87EE-4B9D-AB9A-76BC12E9D097}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{453FA2BB-D8C9-45D5-B1C9-7C5058E34A23}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{C9C9E6DD-8CF5-44D2-96F8-F3FCF9219F54}"/>
-    <hyperlink ref="B20" r:id="rId17" xr:uid="{319ACF75-677F-4C17-9187-E983842E084C}"/>
-    <hyperlink ref="B21" r:id="rId18" xr:uid="{21865637-5EC6-4B26-B97A-2EAE9233FB3D}"/>
-    <hyperlink ref="B23" r:id="rId19" xr:uid="{6BF4CD40-2C25-415A-9A09-4201DB46EDD3}"/>
-    <hyperlink ref="B24" r:id="rId20" xr:uid="{D4EBE406-B66C-462C-B0F7-15C09F9AF805}"/>
-    <hyperlink ref="B25" r:id="rId21" xr:uid="{BE5C11CF-7B2F-42D7-B71C-8EA01919DE80}"/>
-    <hyperlink ref="B26" r:id="rId22" xr:uid="{9A97D4CC-02E6-4BA5-AA0A-3B5E6E5F6EB2}"/>
-    <hyperlink ref="B27" r:id="rId23" xr:uid="{FD3E8A23-2524-4AD9-A02A-D98180A54E10}"/>
-    <hyperlink ref="B28" r:id="rId24" xr:uid="{5F1E5ADD-6E06-430C-A225-EE9B45250578}"/>
-    <hyperlink ref="B29" r:id="rId25" xr:uid="{E15C6FA1-6BBD-4B36-8A8F-FF12721BDD41}"/>
-    <hyperlink ref="B31" r:id="rId26" display="https://www.linkedin.com/in/laxmi-rani-bodana-882436256/recent-activity/documents/" xr:uid="{48DFAD3E-9232-48F3-B79E-3C5E64F6B3E9}"/>
-    <hyperlink ref="B32" r:id="rId27" display="https://www.linkedin.com/in/laxmi-rani-bodana-882436256/recent-activity/documents/" xr:uid="{DF832F82-525F-45A1-B010-0A1FA7C6E5F2}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{0631045F-4915-4FF9-B22B-80AE3126D5B0}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{A4676929-B8C3-4901-8FF5-0BDC3175050E}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{7B7FBE21-B5F8-4EE9-AE85-B2DAD57BCD63}"/>
+    <hyperlink ref="B14" r:id="rId5" display="https://www.linkedin.com/in/laxmi-rani-bodana-882436256/ " xr:uid="{C1C86E05-B6ED-4FCB-960C-C888FC35B72A}"/>
+    <hyperlink ref="B15" r:id="rId6" display="https://github.com/patan-abubakar8" xr:uid="{3B8B51B6-AE2F-4A55-99FC-37BEC1D0E397}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{B2197619-6013-44FB-8DB8-8A25DDCA479F}"/>
+    <hyperlink ref="B17" r:id="rId8" xr:uid="{702632EC-18ED-471F-8542-ECF8E4573F41}"/>
+    <hyperlink ref="B18" r:id="rId9" xr:uid="{B169D8E7-AB76-4F00-BAB8-075FEA5BAA4D}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{15CD9701-331C-4586-B09C-B1A64C71A263}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{B168966D-89E8-4E55-904C-419DDFFE368D}"/>
+    <hyperlink ref="B21" r:id="rId12" xr:uid="{9CB6C6C7-3513-4B06-A3B2-8F63805A5AD0}"/>
+    <hyperlink ref="B22" r:id="rId13" xr:uid="{D20CA113-FD85-4E12-AF69-2E6C5FD5E0C5}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{D306E866-87EE-4B9D-AB9A-76BC12E9D097}"/>
+    <hyperlink ref="B23" r:id="rId15" xr:uid="{453FA2BB-D8C9-45D5-B1C9-7C5058E34A23}"/>
+    <hyperlink ref="B26" r:id="rId16" xr:uid="{C9C9E6DD-8CF5-44D2-96F8-F3FCF9219F54}"/>
+    <hyperlink ref="B27" r:id="rId17" xr:uid="{319ACF75-677F-4C17-9187-E983842E084C}"/>
+    <hyperlink ref="B28" r:id="rId18" xr:uid="{21865637-5EC6-4B26-B97A-2EAE9233FB3D}"/>
+    <hyperlink ref="B30" r:id="rId19" xr:uid="{6BF4CD40-2C25-415A-9A09-4201DB46EDD3}"/>
+    <hyperlink ref="B31" r:id="rId20" xr:uid="{D4EBE406-B66C-462C-B0F7-15C09F9AF805}"/>
+    <hyperlink ref="B32" r:id="rId21" xr:uid="{BE5C11CF-7B2F-42D7-B71C-8EA01919DE80}"/>
+    <hyperlink ref="B33" r:id="rId22" xr:uid="{9A97D4CC-02E6-4BA5-AA0A-3B5E6E5F6EB2}"/>
+    <hyperlink ref="B34" r:id="rId23" xr:uid="{FD3E8A23-2524-4AD9-A02A-D98180A54E10}"/>
+    <hyperlink ref="B35" r:id="rId24" xr:uid="{5F1E5ADD-6E06-430C-A225-EE9B45250578}"/>
+    <hyperlink ref="B37" r:id="rId25" display="https://www.linkedin.com/in/laxmi-rani-bodana-882436256/recent-activity/documents/" xr:uid="{48DFAD3E-9232-48F3-B79E-3C5E64F6B3E9}"/>
+    <hyperlink ref="B38" r:id="rId26" display="https://www.linkedin.com/in/laxmi-rani-bodana-882436256/recent-activity/documents/" xr:uid="{DF832F82-525F-45A1-B010-0A1FA7C6E5F2}"/>
+    <hyperlink ref="B4" r:id="rId27" xr:uid="{5F9A8228-A4CB-4005-9652-F11F17319537}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId28"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671FAD13-2B9A-4FEE-AD72-042A0F2D2EDE}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="173" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>